<commit_message>
Position and style update
</commit_message>
<xml_diff>
--- a/Assets/data.xlsx
+++ b/Assets/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sufy2\Desktop\Collins Signature\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sufy2\Desktop\Collins Signature\Signature\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E7B7CE-ED3E-41A6-BBE9-DDB2002234C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16F01AB-D9CC-464E-858D-032919C9B7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dt" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>testemail@collinsearthworks.co.uk</t>
   </si>
   <si>
-    <t>Ripley DE5</t>
-  </si>
-  <si>
     <t>Designation</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
   </si>
   <si>
     <t>Engineer</t>
-  </si>
-  <si>
-    <t>Collins Earthworks Limited, Whiteley Road, Ripley, Derbyshire, DE5 3QL</t>
   </si>
   <si>
     <t>09876 543210</t>
@@ -920,18 +914,18 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="64.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,10 +942,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -959,19 +953,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -979,19 +970,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
     </row>
   </sheetData>

</xml_diff>